<commit_message>
Minor updates to documentation and scratch
</commit_message>
<xml_diff>
--- a/Database Statistics.xlsx
+++ b/Database Statistics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BT_Lab\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BT_Lab\Documents\RVST598_Speech-Emotion-Recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691098C5-ADCA-4284-9764-2100D33626D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304B465E-1166-417F-8282-D0820FC867E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{98AB058E-348D-4B6A-B9F5-88A9237A336C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Database</t>
   </si>
@@ -41,26 +41,49 @@
     <t>CREMA-D</t>
   </si>
   <si>
-    <t># STD</t>
-  </si>
-  <si>
-    <t># Outliers</t>
-  </si>
-  <si>
-    <t>% Included</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
+    <t>Number of Samples</t>
+  </si>
+  <si>
+    <t>Shortest</t>
+  </si>
+  <si>
+    <t>Longest</t>
+  </si>
+  <si>
+    <t>IEMOCAP</t>
+  </si>
+  <si>
+    <t>TESS</t>
+  </si>
+  <si>
+    <t>EmoV-DB</t>
+  </si>
+  <si>
+    <t>Number of Outliers (&gt; 3 STD)</t>
+  </si>
+  <si>
+    <t>Shortest (after cutoff)</t>
+  </si>
+  <si>
+    <t>Longest (after cutoff)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,22 +93,28 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -96,25 +125,44 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -427,159 +475,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58664C6B-EC5A-44AF-95A6-42D7FC2A6F2F}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.42578125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" s="1">
+        <v>10039</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7442</v>
+      </c>
+      <c r="C3" s="1">
+        <v>70</v>
+      </c>
+      <c r="D3" s="3">
+        <v>60861</v>
+      </c>
+      <c r="E3" s="3">
+        <v>240240</v>
+      </c>
+      <c r="F3" s="3">
+        <v>60861</v>
+      </c>
+      <c r="G3" s="3">
+        <v>193794</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B4" s="1">
+        <v>2800</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>60196</v>
+      </c>
+      <c r="E4" s="3">
+        <v>143271</v>
+      </c>
+      <c r="F4" s="3">
+        <v>60196</v>
+      </c>
+      <c r="G4" s="3">
+        <v>143271</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="5" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2">
+      <c r="B5" s="1">
+        <v>1440</v>
+      </c>
+      <c r="C5" s="1">
         <v>16</v>
       </c>
-      <c r="D2">
-        <f>(1440-C2)/1440</f>
-        <v>0.98888888888888893</v>
-      </c>
-      <c r="E2">
+      <c r="D5" s="3">
         <v>44941</v>
       </c>
-      <c r="F2">
+      <c r="E5" s="3">
+        <v>157053</v>
+      </c>
+      <c r="F5" s="3">
+        <v>44941</v>
+      </c>
+      <c r="G5" s="3">
         <v>128224</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>58</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D6" si="0">(1440-C3)/1440</f>
-        <v>0.95972222222222225</v>
-      </c>
-      <c r="E3">
-        <v>49745</v>
-      </c>
-      <c r="F3">
-        <v>113810</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>425</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
-        <v>0.70486111111111116</v>
-      </c>
-      <c r="E4">
-        <v>65761</v>
-      </c>
-      <c r="F4">
-        <v>96192</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2">
-        <v>70</v>
-      </c>
-      <c r="D5" s="2">
-        <f>(7442-C5)/7442</f>
-        <v>0.99059392636388066</v>
-      </c>
-      <c r="E5" s="2">
-        <v>60861</v>
-      </c>
-      <c r="F5" s="2">
-        <v>193794</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="3">
-        <v>318</v>
-      </c>
-      <c r="D6">
-        <f t="shared" ref="D6:D7" si="1">(7442-C6)/7442</f>
-        <v>0.95726955119591506</v>
-      </c>
-      <c r="E6" s="3">
-        <v>73674</v>
-      </c>
-      <c r="F6" s="3">
-        <v>169770</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3">
-        <v>2228</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="1"/>
-        <v>0.70061811341037361</v>
-      </c>
-      <c r="E7" s="3">
-        <v>99300</v>
-      </c>
-      <c r="F7" s="3">
-        <v>145746</v>
-      </c>
+    <row r="6" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>6599</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Create db_stats and update spreadsheet with stats
</commit_message>
<xml_diff>
--- a/Database Statistics.xlsx
+++ b/Database Statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BT_Lab\Documents\RVST598_Speech-Emotion-Recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{304B465E-1166-417F-8282-D0820FC867E6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1D55B1-44DD-4F2D-B91A-E2E0624A997D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{98AB058E-348D-4B6A-B9F5-88A9237A336C}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -158,7 +158,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -478,7 +478,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>